<commit_message>
Adding in demo for 4 curve tension-pCa fit
</commit_message>
<xml_diff>
--- a/code/demos/fitting/four_curves_tension_pCa/target_data/target_force_pCa_data.xlsx
+++ b/code/demos/fitting/four_curves_tension_pCa/target_data/target_force_pCa_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ken\GitHub\CampbellMuscleLab\models\MATMyoSim\code\demos\fitting\four_curves_tension_pCa\target_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3FFD40-BB5E-4587-968F-FB549728617F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD52681-BC64-41D2-8CE3-6FE2B82D7E83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="1650" windowWidth="24225" windowHeight="13950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="9">
   <si>
     <t>treatment</t>
-  </si>
-  <si>
-    <t>S2_Stabilizing</t>
   </si>
   <si>
     <t>Sham</t>
@@ -46,10 +43,10 @@
     <t>force</t>
   </si>
   <si>
-    <t>force_error</t>
+    <t>curve</t>
   </si>
   <si>
-    <t>curve</t>
+    <t>Drug</t>
   </si>
 </sst>
 </file>
@@ -408,7 +405,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -421,33 +420,31 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <v>6.5</v>
@@ -455,19 +452,16 @@
       <c r="E2">
         <v>436.66666666666669</v>
       </c>
-      <c r="F2">
-        <v>91.802929026136084</v>
-      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>5.8</v>
@@ -475,19 +469,16 @@
       <c r="E3">
         <v>661.11111111111109</v>
       </c>
-      <c r="F3">
-        <v>139.12868188643486</v>
-      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>5.5</v>
@@ -495,19 +486,16 @@
       <c r="E4">
         <v>2231.1111111111113</v>
       </c>
-      <c r="F4">
-        <v>433.73841465297841</v>
-      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>5.4</v>
@@ -515,19 +503,16 @@
       <c r="E5">
         <v>5122.2222222222226</v>
       </c>
-      <c r="F5">
-        <v>818.33295617400972</v>
-      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>5.2</v>
@@ -535,28 +520,22 @@
       <c r="E6">
         <v>13652.222222222223</v>
       </c>
-      <c r="F6">
-        <v>950.45716745179732</v>
-      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>4.8</v>
       </c>
       <c r="E7">
         <v>19701.111111111109</v>
-      </c>
-      <c r="F7">
-        <v>1221.3942902869978</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -564,19 +543,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>6.5</v>
       </c>
       <c r="E8">
         <v>340</v>
-      </c>
-      <c r="F8">
-        <v>149.33184523068078</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -584,19 +560,16 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>5.8</v>
       </c>
       <c r="E9">
         <v>890</v>
-      </c>
-      <c r="F9">
-        <v>389.74350539810155</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -604,19 +577,16 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10">
         <v>5.5</v>
       </c>
       <c r="E10">
         <v>2173.3333333333335</v>
-      </c>
-      <c r="F10">
-        <v>1020.3321899155087</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -624,19 +594,16 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11">
         <v>5.4</v>
       </c>
       <c r="E11">
         <v>3833.3333333333335</v>
-      </c>
-      <c r="F11">
-        <v>1518.1823927900687</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -644,19 +611,16 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12">
         <v>5.2</v>
       </c>
       <c r="E12">
         <v>15243.333333333334</v>
-      </c>
-      <c r="F12">
-        <v>1556.5917183956037</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -664,10 +628,10 @@
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>4.8</v>
@@ -675,19 +639,16 @@
       <c r="E13">
         <v>24403.333333333332</v>
       </c>
-      <c r="F13">
-        <v>2227.0633379208398</v>
-      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14">
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14">
         <v>6.5</v>
@@ -695,19 +656,16 @@
       <c r="E14">
         <v>2063.3333333333335</v>
       </c>
-      <c r="F14">
-        <v>229.53455319648745</v>
-      </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15">
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15">
         <v>5.8</v>
@@ -715,19 +673,16 @@
       <c r="E15">
         <v>3536.6666666666665</v>
       </c>
-      <c r="F15">
-        <v>487.55911322514407</v>
-      </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16">
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16">
         <v>5.5</v>
@@ -735,19 +690,16 @@
       <c r="E16">
         <v>9827.7777777777774</v>
       </c>
-      <c r="F16">
-        <v>1415.0635809996684</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17">
         <v>5.4</v>
@@ -755,19 +707,16 @@
       <c r="E17">
         <v>14632.222222222223</v>
       </c>
-      <c r="F17">
-        <v>1841.5035959310969</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18">
         <v>5.2</v>
@@ -775,19 +724,16 @@
       <c r="E18">
         <v>22434.444444444445</v>
       </c>
-      <c r="F18">
-        <v>1635.5343257982076</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>3</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19">
         <v>4.8</v>
@@ -795,19 +741,16 @@
       <c r="E19">
         <v>24100</v>
       </c>
-      <c r="F19">
-        <v>1380.1871853725736</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20">
         <v>6.5</v>
@@ -815,19 +758,16 @@
       <c r="E20">
         <v>1446.6666666666667</v>
       </c>
-      <c r="F20">
-        <v>256.21171800767519</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D21">
         <v>5.8</v>
@@ -835,19 +775,16 @@
       <c r="E21">
         <v>2303.3333333333335</v>
       </c>
-      <c r="F21">
-        <v>431.29005450057758</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D22">
         <v>5.5</v>
@@ -855,19 +792,16 @@
       <c r="E22">
         <v>4866.666666666667</v>
       </c>
-      <c r="F22">
-        <v>900.78360948182853</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23">
         <v>5.4</v>
@@ -875,19 +809,16 @@
       <c r="E23">
         <v>8593.3333333333339</v>
       </c>
-      <c r="F23">
-        <v>1373.3697406177423</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24">
         <v>5.2</v>
@@ -895,28 +826,22 @@
       <c r="E24">
         <v>21190</v>
       </c>
-      <c r="F24">
-        <v>1232.1931666747712</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D25">
         <v>4.8</v>
       </c>
       <c r="E25">
         <v>26760</v>
-      </c>
-      <c r="F25">
-        <v>1350.0493818128778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>